<commit_message>
with alarm identification page
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -562,9 +562,89 @@
         <v>Increasing</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2024-10-03</v>
+      </c>
+      <c r="B9" t="str">
+        <v>5</v>
+      </c>
+      <c r="C9" t="str">
+        <v>uhf</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Heart Rate</v>
+      </c>
+      <c r="E9" t="str">
+        <v>VeryHigh</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Static</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>2024-10-04</v>
+      </c>
+      <c r="B10" t="str">
+        <v>14</v>
+      </c>
+      <c r="C10" t="str">
+        <v>fr</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Heart Rate</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Low</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Static</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>2024-10-04</v>
+      </c>
+      <c r="B11" t="str">
+        <v>14</v>
+      </c>
+      <c r="C11" t="str">
+        <v>fr</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Oxygen</v>
+      </c>
+      <c r="E11" t="str">
+        <v>High</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Static</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>2024-10-04</v>
+      </c>
+      <c r="B12" t="str">
+        <v>14</v>
+      </c>
+      <c r="C12" t="str">
+        <v>fr</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Blood Pressure</v>
+      </c>
+      <c r="E12" t="str">
+        <v>VeryHigh</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Decreasing</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>